<commit_message>
segunda parte de estandarizacion
</commit_message>
<xml_diff>
--- a/NetApplications/PY/AutomatizacionGestionSolped/Insumo/EnvioCorreos.xlsx
+++ b/NetApplications/PY/AutomatizacionGestionSolped/Insumo/EnvioCorreos.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGRPA009\Documents\SOLPED-main\SOLPED\NetApplications\PY\AutomatizacionGestionSolped\Insumo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0B0E70-F0E1-4554-9DAC-05129A7E44F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="EnvioCorreos"/>
+    <sheet name="EnvioCorreos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -212,8 +218,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -262,41 +267,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -307,10 +309,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -348,71 +350,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -440,7 +442,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -463,11 +465,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -476,13 +478,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -492,7 +494,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -501,7 +503,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -510,7 +512,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -518,10 +520,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -586,28 +588,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="44.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="82.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="82.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,9 +636,8 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="100.5" customFormat="1" s="5">
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -655,12 +658,12 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="73.5" customFormat="1" s="5">
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>13</v>
@@ -668,20 +671,19 @@
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3"/>
+        <v>54</v>
+      </c>
       <c r="I3" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -689,20 +691,19 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="3"/>
+        <v>57</v>
+      </c>
       <c r="I4" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -710,20 +711,20 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -731,20 +732,20 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -752,20 +753,20 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>13</v>
@@ -773,20 +774,20 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -794,20 +795,20 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>10.1785714285714</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>13</v>
@@ -815,20 +816,20 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>11.3571428571429</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>13</v>
@@ -836,20 +837,20 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="60" customFormat="1" s="5">
+    <row r="12" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>12.5357142857143</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>13</v>
@@ -857,20 +858,18 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="60" customFormat="1" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>13.7142857142857</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>13</v>
@@ -878,20 +877,18 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="60" customFormat="1" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>14.8928571428572</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>13</v>
@@ -899,62 +896,20 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="5">
-      <c r="A15" s="1">
-        <v>16.0714285714286</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="5">
-      <c r="A16" s="1">
-        <v>17.25</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="5">
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>18.4285714285715</v>
+        <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>13</v>
@@ -962,13 +917,52 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>